<commit_message>
Changes for reading excel file
Changes for reading excel file
-added a data manager class
-channges for base test
</commit_message>
<xml_diff>
--- a/Resources/Data.xlsx
+++ b/Resources/Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Test01" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>UserName</t>
   </si>
@@ -40,13 +40,37 @@
   </si>
   <si>
     <t>ssmsm</t>
+  </si>
+  <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>MotoX</t>
+  </si>
+  <si>
+    <t>Apple Iphone 6</t>
+  </si>
+  <si>
+    <t>TestA</t>
+  </si>
+  <si>
+    <t>TestB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +78,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,12 +113,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,48 +442,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -429,7 +549,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -441,7 +561,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>